<commit_message>
v0.9 HeliosCap. missing RA motor only
</commit_message>
<xml_diff>
--- a/GearCalculations.xlsx
+++ b/GearCalculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anune\Documents\cosas\Telescope\Heliostat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{219C8B33-CA7F-48C5-B66A-8F88FF8ED2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EAFA58-2647-4EBC-8D25-5179607AC492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D243D50-7BC1-4C4C-8AD6-D574925E227B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>step/grad</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>© Agustin Nunez 2020.  https://github.com/agnunez/HelioCap</t>
+  </si>
+  <si>
+    <t>RAGear</t>
   </si>
 </sst>
 </file>
@@ -241,9 +244,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -254,13 +254,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -269,10 +269,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -589,77 +592,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB6D6F0-3AD6-4A29-9EF2-EBE87C93711E}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>32</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>63.683950000000003</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -673,32 +676,32 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7">
+      <c r="D4" s="4"/>
+      <c r="E4" s="6">
         <f>D3*E3</f>
         <v>2037.8864000000001</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <f>E4/360/C4</f>
         <v>5.6607955555555556</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>1/F4</f>
         <v>0.17665361523586398</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <f>G4*60</f>
         <v>10.599216914151839</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <f>F4*2</f>
         <v>11.321591111111111</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <f>1/I4</f>
         <v>8.8326807617931991E-2</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <f>J4*60</f>
         <v>5.2996084570759194</v>
       </c>
@@ -714,32 +717,32 @@
         <f>B5/A5</f>
         <v>0.2</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7">
+      <c r="D5" s="4"/>
+      <c r="E5" s="6">
         <f>E$4</f>
         <v>2037.8864000000001</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>E5/360/C5</f>
         <v>28.303977777777778</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f>1/F5</f>
         <v>3.5330723047172795E-2</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <f>G5*60</f>
         <v>2.1198433828303678</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <f>F5*2</f>
         <v>56.607955555555556</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f>1/I5</f>
         <v>1.7665361523586397E-2</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <f>J5*60</f>
         <v>1.0599216914151839</v>
       </c>
@@ -755,34 +758,150 @@
         <f>B6/A6</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10">
+      <c r="D6" s="7"/>
+      <c r="E6" s="9">
         <f>E$4</f>
         <v>2037.8864000000001</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f>E6/360/C6</f>
         <v>42.455966666666669</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f>1/F6</f>
         <v>2.3553815364781863E-2</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <f>G6*60</f>
         <v>1.4132289218869118</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <f>F6*2</f>
         <v>84.911933333333337</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <f>1/I6</f>
         <v>1.1776907682390932E-2</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <f>J6*60</f>
         <v>0.70661446094345592</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3">
+        <v>63.683950000000003</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>180</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <f>B9/A9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E9" s="9">
+        <f>E$4</f>
+        <v>2037.8864000000001</v>
+      </c>
+      <c r="F9" s="7">
+        <f>E9/360/C9</f>
+        <v>50.947160000000004</v>
+      </c>
+      <c r="G9" s="8">
+        <f>1/F9</f>
+        <v>1.9628179470651552E-2</v>
+      </c>
+      <c r="H9" s="9">
+        <f>G9*60</f>
+        <v>1.1776907682390931</v>
+      </c>
+      <c r="I9" s="7">
+        <f>F9*2</f>
+        <v>101.89432000000001</v>
+      </c>
+      <c r="J9" s="8">
+        <f>1/I9</f>
+        <v>9.8140897353257758E-3</v>
+      </c>
+      <c r="K9" s="9">
+        <f>J9*60</f>
+        <v>0.58884538411954657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>180</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f>B10/A10</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <f>E$4</f>
+        <v>2037.8864000000001</v>
+      </c>
+      <c r="F10" s="7">
+        <f>E10/360/C10</f>
+        <v>63.683949999999996</v>
+      </c>
+      <c r="G10" s="8">
+        <f>1/F10</f>
+        <v>1.5702543576521243E-2</v>
+      </c>
+      <c r="H10" s="9">
+        <f>G10*60</f>
+        <v>0.94215261459127464</v>
+      </c>
+      <c r="I10" s="7">
+        <f>F10*2</f>
+        <v>127.36789999999999</v>
+      </c>
+      <c r="J10" s="8">
+        <f>1/I10</f>
+        <v>7.8512717882606217E-3</v>
+      </c>
+      <c r="K10" s="9">
+        <f>J10*60</f>
+        <v>0.47107630729563732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>